<commit_message>
text for report 2 broken down
</commit_message>
<xml_diff>
--- a/data-viz/inputs/report_outline_v1.xlsx
+++ b/data-viz/inputs/report_outline_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wjproject.sharepoint.com/research/Programmatic/EU Subnational/EU-S Data/reports/eu-thematic-reports/data-viz/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="543" documentId="13_ncr:1_{3E5CEFF2-10F5-4DCA-8241-20185538709A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB6FA3E4-E335-4729-BCD6-266B5ECED8F2}"/>
+  <xr:revisionPtr revIDLastSave="546" documentId="13_ncr:1_{3E5CEFF2-10F5-4DCA-8241-20185538709A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FACCBE90-7920-48E3-9FB3-82A8C5C72C74}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="16570" windowHeight="11370" xr2:uid="{E4E80D87-C70E-4028-A5D2-942CA65BEF0E}"/>
+    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15720" xr2:uid="{E4E80D87-C70E-4028-A5D2-942CA65BEF0E}"/>
   </bookViews>
   <sheets>
     <sheet name="outline" sheetId="1" r:id="rId1"/>
@@ -4764,43 +4764,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{678B889B-2B8F-47B3-B684-D177E81CA62D}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:W224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R3" sqref="R3"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.1796875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.54296875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.453125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.26953125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="85.54296875" style="1" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="9.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.54296875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="21.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="30.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="34.453125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="16.453125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="8.453125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.453125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="16.453125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="85.5703125" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.5703125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="34.42578125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="16.42578125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="8.42578125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.42578125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="16.42578125" style="1" customWidth="1"/>
     <col min="23" max="23" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="8.54296875" style="1"/>
+    <col min="24" max="16384" width="8.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>983</v>
       </c>
@@ -4871,7 +4870,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -4942,7 +4941,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -5013,7 +5012,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -5084,7 +5083,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -5155,7 +5154,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -5226,7 +5225,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -5297,7 +5296,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -5368,7 +5367,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -5439,7 +5438,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -5510,7 +5509,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -5581,7 +5580,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -5652,7 +5651,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -5723,7 +5722,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -5794,7 +5793,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -5865,7 +5864,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="16" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -5936,7 +5935,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -6007,7 +6006,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="18" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -6078,7 +6077,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="19" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -6149,7 +6148,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="20" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -6220,7 +6219,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="21" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -6291,7 +6290,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="22" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -6362,7 +6361,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -6433,7 +6432,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -6504,7 +6503,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="25" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -6573,7 +6572,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="26" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -6644,7 +6643,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="27" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -6715,7 +6714,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="28" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -6786,7 +6785,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="29" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -6857,7 +6856,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="30" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -6928,7 +6927,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="31" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -6999,7 +6998,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="32" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -7070,7 +7069,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="33" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -7141,7 +7140,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="34" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -7212,7 +7211,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="35" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -7283,7 +7282,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="36" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -7354,7 +7353,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="37" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -7425,7 +7424,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="38" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -7496,7 +7495,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="39" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -7567,7 +7566,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="40" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -7638,7 +7637,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="41" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -7709,7 +7708,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="42" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -7780,7 +7779,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="43" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -7851,7 +7850,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="44" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -7922,7 +7921,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="45" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -7993,7 +7992,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="46" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="10">
         <v>45</v>
       </c>
@@ -8064,7 +8063,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="47" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -8135,7 +8134,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="48" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -8206,7 +8205,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="49" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -8277,7 +8276,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="50" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -8348,7 +8347,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="51" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -8419,7 +8418,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="52" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -8490,7 +8489,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="53" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -8561,7 +8560,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="54" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -8632,7 +8631,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="55" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -8703,7 +8702,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="56" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -8774,7 +8773,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="57" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -8845,7 +8844,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="58" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -8916,7 +8915,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="59" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -8987,7 +8986,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="60" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -9058,7 +9057,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="61" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -9129,7 +9128,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="62" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -9200,7 +9199,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="63" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -9271,7 +9270,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="64" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -9342,7 +9341,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="65" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -9413,7 +9412,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="66" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -9484,7 +9483,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="67" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -9555,7 +9554,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="68" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -9626,7 +9625,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="69" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -9697,7 +9696,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="70" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -9768,7 +9767,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="71" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -9839,7 +9838,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="72" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="10">
         <v>71</v>
       </c>
@@ -9910,7 +9909,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="73" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="10">
         <v>72</v>
       </c>
@@ -9981,7 +9980,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="74" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -10052,7 +10051,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="75" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="26">
         <v>74</v>
       </c>
@@ -10123,7 +10122,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="76" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -10194,7 +10193,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="77" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -10265,7 +10264,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="78" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -10336,7 +10335,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="79" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -10407,7 +10406,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="80" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="26">
         <v>79</v>
       </c>
@@ -10478,7 +10477,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="81" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -10549,7 +10548,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="82" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -10620,7 +10619,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="83" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -10691,7 +10690,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="84" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -10762,7 +10761,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="85" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -10833,7 +10832,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="86" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="10">
         <v>85</v>
       </c>
@@ -10904,7 +10903,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="87" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="10">
         <v>86</v>
       </c>
@@ -10975,7 +10974,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="88" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -11046,7 +11045,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="89" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="10">
         <v>88</v>
       </c>
@@ -11117,7 +11116,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="90" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -11188,7 +11187,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="91" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -11259,7 +11258,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="92" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>91</v>
       </c>
@@ -11330,7 +11329,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="93" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -11401,7 +11400,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="94" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -11472,7 +11471,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="95" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -11543,7 +11542,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="96" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -11614,7 +11613,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="97" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -11685,7 +11684,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="98" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -11756,7 +11755,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="99" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>98</v>
       </c>
@@ -11827,7 +11826,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="100" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>99</v>
       </c>
@@ -11898,7 +11897,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="101" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>100</v>
       </c>
@@ -11969,7 +11968,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="102" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>101</v>
       </c>
@@ -12040,7 +12039,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="103" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>102</v>
       </c>
@@ -12111,7 +12110,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="104" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>103</v>
       </c>
@@ -12182,7 +12181,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="105" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>104</v>
       </c>
@@ -12253,7 +12252,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="106" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>105</v>
       </c>
@@ -12324,7 +12323,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="107" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>106</v>
       </c>
@@ -12395,7 +12394,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="108" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>107</v>
       </c>
@@ -12466,7 +12465,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="109" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>108</v>
       </c>
@@ -12537,7 +12536,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="110" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>109</v>
       </c>
@@ -12608,7 +12607,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="111" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>110</v>
       </c>
@@ -12679,7 +12678,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="112" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>111</v>
       </c>
@@ -12750,7 +12749,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="113" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>112</v>
       </c>
@@ -12821,7 +12820,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="114" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>113</v>
       </c>
@@ -12892,7 +12891,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="115" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>114</v>
       </c>
@@ -12963,7 +12962,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="116" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="10">
         <v>115</v>
       </c>
@@ -13034,7 +13033,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="117" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>116</v>
       </c>
@@ -13105,7 +13104,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="118" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>117</v>
       </c>
@@ -13176,7 +13175,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="119" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>118</v>
       </c>
@@ -13247,7 +13246,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="120" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>119</v>
       </c>
@@ -13318,7 +13317,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="121" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>120</v>
       </c>
@@ -13389,7 +13388,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="122" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>121</v>
       </c>
@@ -13460,7 +13459,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="123" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>122</v>
       </c>
@@ -13531,7 +13530,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="124" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>123</v>
       </c>
@@ -13602,7 +13601,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="125" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>124</v>
       </c>
@@ -13673,7 +13672,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="126" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>125</v>
       </c>
@@ -13744,7 +13743,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="127" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="10">
         <v>126</v>
       </c>
@@ -13815,7 +13814,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="128" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>127</v>
       </c>
@@ -13886,7 +13885,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="129" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>128</v>
       </c>
@@ -13957,7 +13956,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="130" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>129</v>
       </c>
@@ -14028,7 +14027,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="131" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="10">
         <v>130</v>
       </c>
@@ -14099,7 +14098,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="132" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>131</v>
       </c>
@@ -14170,7 +14169,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="133" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>132</v>
       </c>
@@ -14241,7 +14240,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="134" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>133</v>
       </c>
@@ -14312,7 +14311,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="135" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="10">
         <v>134</v>
       </c>
@@ -14383,7 +14382,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="136" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>135</v>
       </c>
@@ -14454,7 +14453,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="137" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>136</v>
       </c>
@@ -14525,7 +14524,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="138" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>137</v>
       </c>
@@ -14596,7 +14595,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="139" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>138</v>
       </c>
@@ -14667,7 +14666,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="140" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>139</v>
       </c>
@@ -14738,7 +14737,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="141" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>140</v>
       </c>
@@ -14809,7 +14808,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="142" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>141</v>
       </c>
@@ -14880,7 +14879,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="143" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>142</v>
       </c>
@@ -14951,7 +14950,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="144" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="10">
         <v>143</v>
       </c>
@@ -15022,7 +15021,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="145" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>144</v>
       </c>
@@ -15093,7 +15092,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="146" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>145</v>
       </c>
@@ -15164,7 +15163,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="147" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>146</v>
       </c>
@@ -15235,7 +15234,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="148" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>147</v>
       </c>
@@ -15306,7 +15305,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="149" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>148</v>
       </c>
@@ -15377,7 +15376,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="150" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>149</v>
       </c>
@@ -15448,7 +15447,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="151" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>150</v>
       </c>
@@ -15519,7 +15518,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="152" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>151</v>
       </c>
@@ -15590,7 +15589,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="153" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="14">
         <v>152</v>
       </c>
@@ -15661,7 +15660,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="154" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>153</v>
       </c>
@@ -15732,7 +15731,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="155" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>154</v>
       </c>
@@ -15803,7 +15802,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="156" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>155</v>
       </c>
@@ -15874,7 +15873,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="157" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>156</v>
       </c>
@@ -15945,7 +15944,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="158" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>158</v>
       </c>
@@ -16016,7 +16015,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="159" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>159</v>
       </c>
@@ -16087,7 +16086,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="160" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>160</v>
       </c>
@@ -16158,7 +16157,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="161" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>161</v>
       </c>
@@ -16229,7 +16228,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="162" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>162</v>
       </c>
@@ -16300,7 +16299,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="163" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>163</v>
       </c>
@@ -16371,7 +16370,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="164" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>164</v>
       </c>
@@ -16442,7 +16441,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="165" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>165</v>
       </c>
@@ -16513,7 +16512,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="166" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>166</v>
       </c>
@@ -16584,7 +16583,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="167" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>167</v>
       </c>
@@ -16655,7 +16654,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="168" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>168</v>
       </c>
@@ -16726,7 +16725,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="169" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>169</v>
       </c>
@@ -16797,7 +16796,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="170" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>170</v>
       </c>
@@ -16868,7 +16867,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="171" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="10">
         <v>171</v>
       </c>
@@ -16939,7 +16938,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="172" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>172</v>
       </c>
@@ -17010,7 +17009,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="173" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>173</v>
       </c>
@@ -17081,7 +17080,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="174" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>174</v>
       </c>
@@ -17152,7 +17151,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="175" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>175</v>
       </c>
@@ -17223,7 +17222,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="176" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>176</v>
       </c>
@@ -17294,7 +17293,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="177" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>177</v>
       </c>
@@ -17365,7 +17364,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="178" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>178</v>
       </c>
@@ -17436,7 +17435,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="179" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>179</v>
       </c>
@@ -17507,7 +17506,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="180" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>180</v>
       </c>
@@ -17578,7 +17577,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="181" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>181</v>
       </c>
@@ -17649,7 +17648,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="182" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>182</v>
       </c>
@@ -17720,7 +17719,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="183" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>183</v>
       </c>
@@ -17791,7 +17790,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="184" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>184</v>
       </c>
@@ -17862,7 +17861,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="185" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>185</v>
       </c>
@@ -17933,7 +17932,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="186" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>186</v>
       </c>
@@ -18004,7 +18003,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="187" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>187</v>
       </c>
@@ -18075,7 +18074,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="188" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="10">
         <v>188</v>
       </c>
@@ -18146,7 +18145,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="189" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>189</v>
       </c>
@@ -18217,7 +18216,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="190" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>190</v>
       </c>
@@ -18288,7 +18287,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="191" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>191</v>
       </c>
@@ -18359,7 +18358,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="192" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="19">
         <v>901</v>
       </c>
@@ -18430,7 +18429,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="193" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="19">
         <v>902</v>
       </c>
@@ -18501,7 +18500,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="194" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="19">
         <v>903</v>
       </c>
@@ -18572,7 +18571,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="195" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="19">
         <v>904</v>
       </c>
@@ -18643,7 +18642,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="196" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="19">
         <v>905</v>
       </c>
@@ -18714,7 +18713,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="197" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="19">
         <v>906</v>
       </c>
@@ -18785,7 +18784,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="198" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="19">
         <v>907</v>
       </c>
@@ -18856,7 +18855,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="199" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="19">
         <v>908</v>
       </c>
@@ -18927,7 +18926,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="200" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="19">
         <v>909</v>
       </c>
@@ -18998,7 +18997,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="201" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="19">
         <v>910</v>
       </c>
@@ -19069,7 +19068,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="202" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="19">
         <v>911</v>
       </c>
@@ -19140,7 +19139,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="203" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="19">
         <v>912</v>
       </c>
@@ -19211,7 +19210,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="204" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="19">
         <v>913</v>
       </c>
@@ -19282,7 +19281,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="205" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="19">
         <v>914</v>
       </c>
@@ -19353,7 +19352,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="206" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="19">
         <v>915</v>
       </c>
@@ -19422,7 +19421,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="207" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="19">
         <v>916</v>
       </c>
@@ -19491,7 +19490,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="208" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="19">
         <v>917</v>
       </c>
@@ -19562,7 +19561,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="209" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="19">
         <v>918</v>
       </c>
@@ -19633,7 +19632,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="210" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="19">
         <v>919</v>
       </c>
@@ -19704,7 +19703,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="211" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="19">
         <v>920</v>
       </c>
@@ -19775,7 +19774,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="212" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="19">
         <v>921</v>
       </c>
@@ -19846,7 +19845,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="213" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="19">
         <v>922</v>
       </c>
@@ -19917,7 +19916,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="214" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="19">
         <v>923</v>
       </c>
@@ -19988,7 +19987,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="215" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="19">
         <v>924</v>
       </c>
@@ -20059,7 +20058,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="216" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="19">
         <v>925</v>
       </c>
@@ -20130,7 +20129,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="217" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="19">
         <v>926</v>
       </c>
@@ -20201,7 +20200,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="218" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="19">
         <v>927</v>
       </c>
@@ -20272,7 +20271,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="219" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="19">
         <v>928</v>
       </c>
@@ -20343,7 +20342,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="220" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="19">
         <v>929</v>
       </c>
@@ -20414,7 +20413,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="221" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="19">
         <v>930</v>
       </c>
@@ -20485,7 +20484,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="222" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="19">
         <v>931</v>
       </c>
@@ -20556,7 +20555,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="223" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="19">
         <v>932</v>
       </c>
@@ -20627,7 +20626,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="224" spans="1:23" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="19">
         <v>933</v>
       </c>
@@ -20699,24 +20698,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:W224" xr:uid="{678B889B-2B8F-47B3-B684-D177E81CA62D}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Democracy &amp; Fundamental Rights"/>
-        <filter val="Transparency &amp; Corruption"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="4">
-      <filters>
-        <filter val="TRUE"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="5">
-      <filters>
-        <filter val="QRQ"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:W224" xr:uid="{678B889B-2B8F-47B3-B684-D177E81CA62D}"/>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="K24:K32">
     <cfRule type="duplicateValues" dxfId="21" priority="26"/>
@@ -20790,17 +20772,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="46f3a809-46a3-44ee-a0f1-42a271529c86">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="69276225-f05c-44c5-92dc-c999460a4149" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006BF094976B1C6245BAB5BCECAC284645" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3620e9c0d1a16779aea146adda0186f7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="69276225-f05c-44c5-92dc-c999460a4149" xmlns:ns3="46f3a809-46a3-44ee-a0f1-42a271529c86" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f2afd3ea0446edf26a13b3c7fc9e6232" ns2:_="" ns3:_="">
     <xsd:import namespace="69276225-f05c-44c5-92dc-c999460a4149"/>
@@ -21049,6 +21020,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="46f3a809-46a3-44ee-a0f1-42a271529c86">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="69276225-f05c-44c5-92dc-c999460a4149" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -21059,23 +21041,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C90AEE68-61A6-4BF6-BC85-1C02B4CC1F94}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="46f3a809-46a3-44ee-a0f1-42a271529c86"/>
-    <ds:schemaRef ds:uri="69276225-f05c-44c5-92dc-c999460a4149"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB09E8AE-AF03-40F5-838A-EED1C518F65A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -21094,6 +21059,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C90AEE68-61A6-4BF6-BC85-1C02B4CC1F94}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="46f3a809-46a3-44ee-a0f1-42a271529c86"/>
+    <ds:schemaRef ds:uri="69276225-f05c-44c5-92dc-c999460a4149"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA55028A-08FA-4D39-ACFA-8A6E9119216A}">
   <ds:schemaRefs>

</xml_diff>